<commit_message>
Updated CO2 script and data files from sharedrive
</commit_message>
<xml_diff>
--- a/data/Bi-weekly_Tank_Sampling_2023.xlsx
+++ b/data/Bi-weekly_Tank_Sampling_2023.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl-my.sharepoint.com/personal/finnegan_roach_pnnl_gov/Documents/Documents/GitHub/mcdr_mesocosm_sensors/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\2023\Eelgrass_Mesocosm\Data_Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{55BF5860-81BE-4FC2-A035-4F5A08166667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50EE8EB6-86BF-4757-ADAF-71A9F0D80970}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA6BCF1-AC4C-42AA-B47B-543003DC3C28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="690" windowWidth="16800" windowHeight="9510" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="META" sheetId="1" r:id="rId1"/>
@@ -335,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -401,16 +401,15 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -753,9 +752,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CB21E28-2209-458E-B639-7E39D56BC310}">
   <dimension ref="A1:P86"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E63" sqref="E63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -780,7 +779,7 @@
       <c r="B1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="27" t="s">
         <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -825,7 +824,7 @@
       <c r="B2" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="27">
+      <c r="C2" s="28">
         <v>0.56944444444444442</v>
       </c>
       <c r="D2" s="12">
@@ -868,7 +867,7 @@
       <c r="B3" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="27">
+      <c r="C3" s="28">
         <v>0.56597222222222221</v>
       </c>
       <c r="D3" s="12">
@@ -907,7 +906,7 @@
     <row r="4" spans="1:16" s="15" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
-      <c r="C4" s="27"/>
+      <c r="C4" s="28"/>
       <c r="D4" s="12"/>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
@@ -928,7 +927,7 @@
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="28">
+      <c r="C5" s="29">
         <v>0.57152777777777775</v>
       </c>
       <c r="D5">
@@ -973,7 +972,7 @@
       <c r="B6" s="3">
         <v>1</v>
       </c>
-      <c r="C6" s="28">
+      <c r="C6" s="29">
         <v>0.55347222222222225</v>
       </c>
       <c r="D6" s="20">
@@ -1016,7 +1015,7 @@
       <c r="B7" s="3">
         <v>2</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C7" s="29">
         <v>0.55833333333333335</v>
       </c>
       <c r="D7" s="20">
@@ -1059,7 +1058,7 @@
       <c r="B8" s="3">
         <v>3</v>
       </c>
-      <c r="C8" s="28">
+      <c r="C8" s="29">
         <v>0.56319444444444444</v>
       </c>
       <c r="D8" s="20">
@@ -1102,7 +1101,7 @@
       <c r="B9" s="3">
         <v>4</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C9" s="29">
         <v>0.55625000000000002</v>
       </c>
       <c r="D9" s="20">
@@ -1145,7 +1144,7 @@
       <c r="B10" s="3">
         <v>5</v>
       </c>
-      <c r="C10" s="28">
+      <c r="C10" s="29">
         <v>0.54861111111111105</v>
       </c>
       <c r="D10" s="20">
@@ -1188,7 +1187,7 @@
       <c r="B11" s="3">
         <v>6</v>
       </c>
-      <c r="C11" s="28">
+      <c r="C11" s="29">
         <v>0.54166666666666663</v>
       </c>
       <c r="D11" s="20">
@@ -1231,7 +1230,7 @@
       <c r="B12" s="3">
         <v>7</v>
       </c>
-      <c r="C12" s="28">
+      <c r="C12" s="29">
         <v>0.53333333333333333</v>
       </c>
       <c r="D12" s="20">
@@ -1274,7 +1273,7 @@
       <c r="B13" s="3">
         <v>8</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="29" t="s">
         <v>41</v>
       </c>
       <c r="D13" s="20">
@@ -1315,7 +1314,7 @@
       <c r="B14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="28">
+      <c r="C14" s="29">
         <v>0.5229166666666667</v>
       </c>
       <c r="D14">
@@ -1350,7 +1349,7 @@
       <c r="B15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="29" t="s">
         <v>42</v>
       </c>
       <c r="J15" s="4"/>
@@ -1371,7 +1370,7 @@
       <c r="B16" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="28">
+      <c r="C16" s="29">
         <v>0.42638888888888887</v>
       </c>
       <c r="D16" s="20">
@@ -1414,7 +1413,7 @@
       <c r="B17" s="3">
         <v>1</v>
       </c>
-      <c r="C17" s="28">
+      <c r="C17" s="29">
         <v>0.42152777777777778</v>
       </c>
       <c r="D17" s="20">
@@ -1455,7 +1454,7 @@
       <c r="B18" s="3">
         <v>2</v>
       </c>
-      <c r="C18" s="28">
+      <c r="C18" s="29">
         <v>0.4201388888888889</v>
       </c>
       <c r="D18" s="20">
@@ -1496,7 +1495,7 @@
       <c r="B19" s="3">
         <v>3</v>
       </c>
-      <c r="C19" s="28">
+      <c r="C19" s="29">
         <v>0.41666666666666669</v>
       </c>
       <c r="D19" s="20">
@@ -1537,7 +1536,7 @@
       <c r="B20" s="3">
         <v>4</v>
       </c>
-      <c r="C20" s="28">
+      <c r="C20" s="29">
         <v>0.41388888888888892</v>
       </c>
       <c r="D20" s="20">
@@ -1578,7 +1577,7 @@
       <c r="B21" s="3">
         <v>5</v>
       </c>
-      <c r="C21" s="28">
+      <c r="C21" s="29">
         <v>0.41041666666666665</v>
       </c>
       <c r="D21" s="20">
@@ -1619,7 +1618,7 @@
       <c r="B22" s="3">
         <v>6</v>
       </c>
-      <c r="C22" s="28">
+      <c r="C22" s="29">
         <v>0.40625</v>
       </c>
       <c r="D22" s="20">
@@ -1660,7 +1659,7 @@
       <c r="B23" s="3">
         <v>7</v>
       </c>
-      <c r="C23" s="28">
+      <c r="C23" s="29">
         <v>0.40416666666666662</v>
       </c>
       <c r="D23" s="20">
@@ -1701,7 +1700,7 @@
       <c r="B24" s="3">
         <v>8</v>
       </c>
-      <c r="C24" s="28">
+      <c r="C24" s="29">
         <v>0.39999999999999997</v>
       </c>
       <c r="D24" s="20">
@@ -1742,7 +1741,7 @@
       <c r="B25" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="28">
+      <c r="C25" s="29">
         <v>0.39583333333333331</v>
       </c>
       <c r="D25">
@@ -1777,7 +1776,7 @@
       <c r="B26" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="28"/>
+      <c r="C26" s="29"/>
       <c r="D26" s="20">
         <v>394.6</v>
       </c>
@@ -1810,7 +1809,7 @@
       <c r="B27" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="28">
+      <c r="C27" s="29">
         <v>0.66388888888888886</v>
       </c>
       <c r="D27" s="20">
@@ -1855,7 +1854,7 @@
       <c r="B28" s="3">
         <v>1</v>
       </c>
-      <c r="C28" s="28">
+      <c r="C28" s="29">
         <v>0.65833333333333333</v>
       </c>
       <c r="D28" s="20">
@@ -1898,7 +1897,7 @@
       <c r="B29" s="3">
         <v>2</v>
       </c>
-      <c r="C29" s="28">
+      <c r="C29" s="29">
         <v>0.65763888888888888</v>
       </c>
       <c r="D29" s="20">
@@ -1941,7 +1940,7 @@
       <c r="B30" s="3">
         <v>3</v>
       </c>
-      <c r="C30" s="28">
+      <c r="C30" s="29">
         <v>0.65208333333333335</v>
       </c>
       <c r="D30" s="20">
@@ -1984,7 +1983,7 @@
       <c r="B31" s="3">
         <v>4</v>
       </c>
-      <c r="C31" s="28">
+      <c r="C31" s="29">
         <v>0.65069444444444446</v>
       </c>
       <c r="D31" s="20">
@@ -2027,7 +2026,7 @@
       <c r="B32" s="3">
         <v>5</v>
       </c>
-      <c r="C32" s="28">
+      <c r="C32" s="29">
         <v>0.64722222222222225</v>
       </c>
       <c r="D32" s="20">
@@ -2070,7 +2069,7 @@
       <c r="B33" s="3">
         <v>6</v>
       </c>
-      <c r="C33" s="28">
+      <c r="C33" s="29">
         <v>0.64374999999999993</v>
       </c>
       <c r="D33" s="20">
@@ -2115,7 +2114,7 @@
       <c r="B34" s="3">
         <v>7</v>
       </c>
-      <c r="C34" s="28">
+      <c r="C34" s="29">
         <v>0.64027777777777783</v>
       </c>
       <c r="D34" s="20">
@@ -2160,7 +2159,7 @@
       <c r="B35" s="3">
         <v>8</v>
       </c>
-      <c r="C35" s="28">
+      <c r="C35" s="29">
         <v>0.63680555555555551</v>
       </c>
       <c r="D35" s="20">
@@ -2203,7 +2202,7 @@
       <c r="B36" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C36" s="28">
+      <c r="C36" s="29">
         <v>0.62777777777777777</v>
       </c>
       <c r="D36" s="9">
@@ -2240,7 +2239,7 @@
       <c r="B37" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C37" s="28">
+      <c r="C37" s="29">
         <v>0.62777777777777777</v>
       </c>
       <c r="D37" s="9">
@@ -2277,7 +2276,7 @@
       <c r="B38" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C38" s="28">
+      <c r="C38" s="29">
         <v>0.68402777777777779</v>
       </c>
       <c r="D38" s="20">
@@ -2314,7 +2313,7 @@
       <c r="B39" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C39" s="28">
+      <c r="C39" s="29">
         <v>0.43263888888888885</v>
       </c>
       <c r="D39" s="20">
@@ -2357,7 +2356,7 @@
       <c r="B40" s="3">
         <v>1</v>
       </c>
-      <c r="C40" s="28">
+      <c r="C40" s="29">
         <v>0.42986111111111108</v>
       </c>
       <c r="D40">
@@ -2400,7 +2399,7 @@
       <c r="B41" s="3">
         <v>2</v>
       </c>
-      <c r="C41" s="28">
+      <c r="C41" s="29">
         <v>0.42569444444444443</v>
       </c>
       <c r="D41">
@@ -2443,7 +2442,7 @@
       <c r="B42" s="3">
         <v>3</v>
       </c>
-      <c r="C42" s="28">
+      <c r="C42" s="29">
         <v>0.43263888888888885</v>
       </c>
       <c r="D42">
@@ -2486,7 +2485,7 @@
       <c r="B43" s="3">
         <v>4</v>
       </c>
-      <c r="C43" s="28">
+      <c r="C43" s="29">
         <v>0.4236111111111111</v>
       </c>
       <c r="D43">
@@ -2529,7 +2528,7 @@
       <c r="B44" s="3">
         <v>5</v>
       </c>
-      <c r="C44" s="28">
+      <c r="C44" s="29">
         <v>0.4201388888888889</v>
       </c>
       <c r="D44">
@@ -2572,7 +2571,7 @@
       <c r="B45" s="3">
         <v>6</v>
       </c>
-      <c r="C45" s="28">
+      <c r="C45" s="29">
         <v>0.41597222222222219</v>
       </c>
       <c r="D45">
@@ -2615,7 +2614,7 @@
       <c r="B46" s="3">
         <v>7</v>
       </c>
-      <c r="C46" s="28">
+      <c r="C46" s="29">
         <v>0.4152777777777778</v>
       </c>
       <c r="D46">
@@ -2658,7 +2657,7 @@
       <c r="B47" s="3">
         <v>8</v>
       </c>
-      <c r="C47" s="28">
+      <c r="C47" s="29">
         <v>0.41319444444444442</v>
       </c>
       <c r="D47">
@@ -2701,7 +2700,7 @@
       <c r="B48" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C48" s="28"/>
+      <c r="C48" s="29"/>
       <c r="D48">
         <v>416.4</v>
       </c>
@@ -2738,7 +2737,7 @@
       <c r="B49" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C49" s="28"/>
+      <c r="C49" s="29"/>
       <c r="D49">
         <v>412.3</v>
       </c>
@@ -2775,7 +2774,7 @@
       <c r="B50" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C50" s="28">
+      <c r="C50" s="29">
         <v>0.40902777777777777</v>
       </c>
       <c r="D50">
@@ -2806,10 +2805,33 @@
       <c r="P50" s="4"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A51" s="16">
+        <v>45110</v>
+      </c>
       <c r="B51" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C51" s="28"/>
+      <c r="C51" s="29">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="D51">
+        <v>495.1</v>
+      </c>
+      <c r="E51" s="21">
+        <v>0.40279999999999999</v>
+      </c>
+      <c r="F51" s="21">
+        <v>0.59689999999999999</v>
+      </c>
+      <c r="G51" s="21">
+        <v>3.101E-3</v>
+      </c>
+      <c r="H51" s="21">
+        <v>5.8079999999999998</v>
+      </c>
+      <c r="I51" s="21">
+        <v>6.4180000000000001E-3</v>
+      </c>
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
       <c r="L51" s="4"/>
@@ -2818,10 +2840,33 @@
       <c r="P51" s="4"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A52" s="16">
+        <v>45110</v>
+      </c>
       <c r="B52" s="3">
         <v>1</v>
       </c>
-      <c r="C52" s="28"/>
+      <c r="C52" s="29">
+        <v>0.57361111111111118</v>
+      </c>
+      <c r="D52">
+        <v>310.60000000000002</v>
+      </c>
+      <c r="E52">
+        <v>0.63360000000000005</v>
+      </c>
+      <c r="F52">
+        <v>0.54410000000000003</v>
+      </c>
+      <c r="G52">
+        <v>6.5599999999999999E-3</v>
+      </c>
+      <c r="H52">
+        <v>8.92</v>
+      </c>
+      <c r="I52">
+        <v>1.7309999999999999E-2</v>
+      </c>
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
       <c r="L52" s="4"/>
@@ -2830,10 +2875,33 @@
       <c r="P52" s="4"/>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A53" s="16">
+        <v>45110</v>
+      </c>
       <c r="B53" s="3">
         <v>2</v>
       </c>
-      <c r="C53" s="28"/>
+      <c r="C53" s="29">
+        <v>0.56805555555555554</v>
+      </c>
+      <c r="D53">
+        <v>399</v>
+      </c>
+      <c r="E53">
+        <v>0.84950000000000003</v>
+      </c>
+      <c r="F53">
+        <v>0.51419999999999999</v>
+      </c>
+      <c r="G53">
+        <v>3.3E-3</v>
+      </c>
+      <c r="H53">
+        <v>8.0220000000000002</v>
+      </c>
+      <c r="I53">
+        <v>2.5180000000000001E-2</v>
+      </c>
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
       <c r="L53" s="4"/>
@@ -2842,10 +2910,33 @@
       <c r="P53" s="4"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A54" s="16">
+        <v>45110</v>
+      </c>
       <c r="B54" s="3">
         <v>3</v>
       </c>
-      <c r="C54" s="28"/>
+      <c r="C54" s="29">
+        <v>0.56805555555555554</v>
+      </c>
+      <c r="D54">
+        <v>381.8</v>
+      </c>
+      <c r="E54">
+        <v>2.3919999999999999</v>
+      </c>
+      <c r="F54">
+        <v>0.52729999999999999</v>
+      </c>
+      <c r="G54">
+        <v>5.9319999999999998E-3</v>
+      </c>
+      <c r="H54">
+        <v>5.9249999999999998</v>
+      </c>
+      <c r="I54">
+        <v>1.0840000000000001E-2</v>
+      </c>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
@@ -2854,118 +2945,302 @@
       <c r="P54" s="4"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A55" s="16">
+        <v>45110</v>
+      </c>
       <c r="B55" s="3">
         <v>4</v>
       </c>
-      <c r="C55" s="28"/>
+      <c r="C55" s="29">
+        <v>0.56597222222222221</v>
+      </c>
+      <c r="D55">
+        <v>235.2</v>
+      </c>
+      <c r="E55">
+        <v>0.78459999999999996</v>
+      </c>
+      <c r="F55">
+        <v>0.5212</v>
+      </c>
+      <c r="G55">
+        <v>3.8769999999999998E-3</v>
+      </c>
+      <c r="H55">
+        <v>11.19</v>
+      </c>
+      <c r="I55">
+        <v>1.8100000000000002E-2</v>
+      </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A56" s="16">
+        <v>45110</v>
+      </c>
       <c r="B56" s="3">
         <v>5</v>
       </c>
-      <c r="C56" s="28"/>
+      <c r="C56" s="29">
+        <v>0.5625</v>
+      </c>
+      <c r="D56">
+        <v>542.4</v>
+      </c>
+      <c r="E56">
+        <v>1.456</v>
+      </c>
+      <c r="F56">
+        <v>0.52990000000000004</v>
+      </c>
+      <c r="G56">
+        <v>4.2069999999999998E-3</v>
+      </c>
+      <c r="H56">
+        <v>7.0110000000000001</v>
+      </c>
+      <c r="I56">
+        <v>8.5979999999999997E-3</v>
+      </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A57" s="16">
+        <v>45110</v>
+      </c>
       <c r="B57" s="3">
         <v>6</v>
       </c>
-      <c r="C57" s="28"/>
+      <c r="C57" s="29">
+        <v>0.56180555555555556</v>
+      </c>
+      <c r="D57">
+        <v>293.89999999999998</v>
+      </c>
+      <c r="E57">
+        <v>0.89359999999999995</v>
+      </c>
+      <c r="F57">
+        <v>0.53810000000000002</v>
+      </c>
+      <c r="G57">
+        <v>4.4689999999999999E-3</v>
+      </c>
+      <c r="H57">
+        <v>6.22</v>
+      </c>
+      <c r="I57">
+        <v>4.5059999999999996E-3</v>
+      </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A58" s="16">
+        <v>45110</v>
+      </c>
       <c r="B58" s="3">
         <v>7</v>
       </c>
-      <c r="C58" s="28"/>
+      <c r="C58" s="29">
+        <v>0.55694444444444446</v>
+      </c>
+      <c r="D58">
+        <v>366</v>
+      </c>
+      <c r="E58">
+        <v>1.196</v>
+      </c>
+      <c r="F58">
+        <v>0.52229999999999999</v>
+      </c>
+      <c r="G58">
+        <v>5.0029999999999996E-3</v>
+      </c>
+      <c r="H58">
+        <v>9.0969999999999995</v>
+      </c>
+      <c r="I58">
+        <v>1.0749999999999999E-2</v>
+      </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A59" s="16">
+        <v>45110</v>
+      </c>
       <c r="B59" s="3">
         <v>8</v>
       </c>
-      <c r="C59" s="28"/>
+      <c r="C59" s="29">
+        <v>0.55763888888888891</v>
+      </c>
+      <c r="D59">
+        <v>469.3</v>
+      </c>
+      <c r="E59">
+        <v>0.78649999999999998</v>
+      </c>
+      <c r="F59">
+        <v>0.53039999999999998</v>
+      </c>
+      <c r="G59">
+        <v>3.156E-3</v>
+      </c>
+      <c r="H59">
+        <v>7.9539999999999997</v>
+      </c>
+      <c r="I59">
+        <v>2.9100000000000001E-2</v>
+      </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A60" s="16">
+        <v>45110</v>
+      </c>
       <c r="B60" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C60" s="28"/>
+      <c r="C60" s="29">
+        <v>0.58194444444444449</v>
+      </c>
+      <c r="D60">
+        <v>417.8</v>
+      </c>
+      <c r="E60">
+        <v>1.53</v>
+      </c>
+      <c r="F60">
+        <v>2.9919999999999999E-2</v>
+      </c>
+      <c r="G60">
+        <v>5.3280000000000003E-3</v>
+      </c>
+      <c r="H60">
+        <v>0.12590000000000001</v>
+      </c>
+      <c r="I60">
+        <v>5.1650000000000003E-3</v>
+      </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A61" s="16">
+        <v>45110</v>
+      </c>
       <c r="B61" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C61" s="28"/>
+      <c r="C61" s="29">
+        <v>0.60277777777777775</v>
+      </c>
+      <c r="D61">
+        <v>411.9</v>
+      </c>
+      <c r="E61">
+        <v>2.1</v>
+      </c>
+      <c r="F61">
+        <v>5.509E-2</v>
+      </c>
+      <c r="G61">
+        <v>5.8640000000000003E-3</v>
+      </c>
+      <c r="H61">
+        <v>0.17949999999999999</v>
+      </c>
+      <c r="I61">
+        <v>1.225E-2</v>
+      </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A62" s="16">
+        <v>45110</v>
+      </c>
       <c r="B62" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C62" s="28"/>
+      <c r="C62" s="29">
+        <v>0.55833333333333335</v>
+      </c>
+      <c r="D62">
+        <v>416.1</v>
+      </c>
+      <c r="E62">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="F62">
+        <v>0.36759999999999998</v>
+      </c>
+      <c r="G62">
+        <v>5.1359999999999999E-3</v>
+      </c>
+      <c r="H62">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="I62">
+        <v>5.0870000000000004E-3</v>
+      </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B63" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C63" s="28"/>
+      <c r="C63" s="29"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B64" s="3">
         <v>1</v>
       </c>
-      <c r="C64" s="28"/>
+      <c r="C64" s="29"/>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B65" s="3">
         <v>2</v>
       </c>
-      <c r="C65" s="28"/>
+      <c r="C65" s="29"/>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B66" s="3">
         <v>3</v>
       </c>
-      <c r="C66" s="28"/>
+      <c r="C66" s="29"/>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B67" s="3">
         <v>4</v>
       </c>
-      <c r="C67" s="28"/>
+      <c r="C67" s="17"/>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B68" s="3">
         <v>5</v>
       </c>
-      <c r="C68" s="28"/>
+      <c r="C68" s="17"/>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B69" s="3">
         <v>6</v>
       </c>
-      <c r="C69" s="28"/>
+      <c r="C69" s="17"/>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B70" s="3">
         <v>7</v>
       </c>
-      <c r="C70" s="28"/>
+      <c r="C70" s="17"/>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B71" s="3">
         <v>8</v>
       </c>
-      <c r="C71" s="28"/>
+      <c r="C71" s="17"/>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B72" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C72" s="28"/>
+      <c r="C72" s="17"/>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B73" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C73" s="28"/>
+      <c r="C73" s="17"/>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B74" s="3" t="s">
@@ -3411,10 +3686,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{219CC811-8442-4429-81C5-6ADB9C52A9AC}">
-  <dimension ref="A1:N40"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3431,7 +3706,7 @@
       <c r="B1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="18" t="s">
         <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -3475,7 +3750,7 @@
       <c r="B2">
         <v>3</v>
       </c>
-      <c r="C2" s="30">
+      <c r="C2" s="22">
         <v>0.44097222222222227</v>
       </c>
       <c r="D2">
@@ -3516,7 +3791,7 @@
       <c r="B3">
         <v>5</v>
       </c>
-      <c r="C3" s="30">
+      <c r="C3" s="22">
         <v>0.44513888888888892</v>
       </c>
       <c r="D3">
@@ -3557,7 +3832,7 @@
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" s="30">
+      <c r="C4" s="22">
         <v>0.46388888888888885</v>
       </c>
       <c r="D4">
@@ -3599,7 +3874,7 @@
       <c r="B5">
         <v>5</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="22">
         <v>0.46319444444444446</v>
       </c>
       <c r="D5">
@@ -3641,7 +3916,7 @@
       <c r="B6">
         <v>3</v>
       </c>
-      <c r="C6" s="30">
+      <c r="C6" s="22">
         <v>0.48680555555555555</v>
       </c>
       <c r="D6">
@@ -3683,7 +3958,7 @@
       <c r="B7">
         <v>5</v>
       </c>
-      <c r="C7" s="30">
+      <c r="C7" s="22">
         <v>0.48472222222222222</v>
       </c>
       <c r="D7">
@@ -3725,7 +4000,7 @@
       <c r="B8">
         <v>3</v>
       </c>
-      <c r="C8" s="30">
+      <c r="C8" s="22">
         <v>0.50555555555555554</v>
       </c>
       <c r="D8">
@@ -3767,7 +4042,7 @@
       <c r="B9">
         <v>5</v>
       </c>
-      <c r="C9" s="30">
+      <c r="C9" s="22">
         <v>0.50486111111111109</v>
       </c>
       <c r="D9">
@@ -3809,7 +4084,7 @@
       <c r="B10">
         <v>3</v>
       </c>
-      <c r="C10" s="30">
+      <c r="C10" s="22">
         <v>0.52430555555555558</v>
       </c>
       <c r="D10">
@@ -3851,7 +4126,7 @@
       <c r="B11">
         <v>5</v>
       </c>
-      <c r="C11" s="30">
+      <c r="C11" s="22">
         <v>0.52430555555555558</v>
       </c>
       <c r="D11">
@@ -3893,7 +4168,7 @@
       <c r="B12">
         <v>3</v>
       </c>
-      <c r="C12" s="30">
+      <c r="C12" s="22">
         <v>0.54027777777777775</v>
       </c>
       <c r="D12">
@@ -3935,7 +4210,7 @@
       <c r="B13">
         <v>5</v>
       </c>
-      <c r="C13" s="30">
+      <c r="C13" s="22">
         <v>0.54166666666666663</v>
       </c>
       <c r="D13">
@@ -3977,7 +4252,7 @@
       <c r="B14" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="30">
+      <c r="C14" s="22">
         <v>407.5</v>
       </c>
       <c r="D14">
@@ -4009,7 +4284,7 @@
       <c r="B15" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="30">
+      <c r="C15" s="22">
         <v>0.55138888888888882</v>
       </c>
       <c r="D15">
@@ -4041,7 +4316,7 @@
       <c r="B16" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="30">
+      <c r="C16" s="22">
         <v>0.41666666666666669</v>
       </c>
       <c r="D16">
@@ -4070,7 +4345,7 @@
       <c r="B17" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="30">
+      <c r="C17" s="22">
         <v>0.62430555555555556</v>
       </c>
       <c r="D17">
@@ -4105,7 +4380,7 @@
       <c r="B18" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="30">
+      <c r="C18" s="22">
         <v>0.62430555555555556</v>
       </c>
       <c r="D18">
@@ -4140,7 +4415,7 @@
       <c r="B19">
         <v>3</v>
       </c>
-      <c r="C19" s="30">
+      <c r="C19" s="22">
         <v>0.54791666666666672</v>
       </c>
       <c r="D19">
@@ -4184,7 +4459,7 @@
       <c r="B20">
         <v>5</v>
       </c>
-      <c r="C20" s="30">
+      <c r="C20" s="22">
         <v>0.54652777777777783</v>
       </c>
       <c r="D20">
@@ -4228,7 +4503,7 @@
       <c r="B21">
         <v>3</v>
       </c>
-      <c r="C21" s="30">
+      <c r="C21" s="22">
         <v>0.64027777777777783</v>
       </c>
       <c r="D21">
@@ -4269,7 +4544,7 @@
       <c r="B22">
         <v>5</v>
       </c>
-      <c r="C22" s="30">
+      <c r="C22" s="22">
         <v>0.63750000000000007</v>
       </c>
       <c r="D22">
@@ -4310,7 +4585,7 @@
       <c r="B23">
         <v>3</v>
       </c>
-      <c r="C23" s="30">
+      <c r="C23" s="22">
         <v>0.65486111111111112</v>
       </c>
       <c r="D23">
@@ -4351,7 +4626,7 @@
       <c r="B24">
         <v>5</v>
       </c>
-      <c r="C24" s="30">
+      <c r="C24" s="22">
         <v>0.65347222222222223</v>
       </c>
       <c r="D24">
@@ -4392,7 +4667,7 @@
       <c r="B25" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="30">
+      <c r="C25" s="22">
         <v>0.54722222222222217</v>
       </c>
       <c r="D25">
@@ -4427,7 +4702,7 @@
       <c r="B26" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="30">
+      <c r="C26" s="22">
         <v>0.62708333333333333</v>
       </c>
       <c r="D26">
@@ -4462,7 +4737,7 @@
       <c r="B27" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="30">
+      <c r="C27" s="22">
         <v>0.54861111111111105</v>
       </c>
       <c r="D27">
@@ -4494,7 +4769,7 @@
       <c r="B28">
         <v>3</v>
       </c>
-      <c r="C28" s="30">
+      <c r="C28" s="22">
         <v>0.55625000000000002</v>
       </c>
       <c r="D28">
@@ -4535,7 +4810,7 @@
       <c r="B29">
         <v>5</v>
       </c>
-      <c r="C29" s="30">
+      <c r="C29" s="22">
         <v>0.55763888888888891</v>
       </c>
       <c r="D29">
@@ -4576,7 +4851,7 @@
       <c r="B30">
         <v>3</v>
       </c>
-      <c r="C30" s="30">
+      <c r="C30" s="22">
         <v>0.56597222222222221</v>
       </c>
       <c r="D30">
@@ -4617,7 +4892,7 @@
       <c r="B31">
         <v>5</v>
       </c>
-      <c r="C31" s="30">
+      <c r="C31" s="22">
         <v>0.56944444444444442</v>
       </c>
       <c r="D31">
@@ -4658,7 +4933,7 @@
       <c r="B32">
         <v>3</v>
       </c>
-      <c r="C32" s="30">
+      <c r="C32" s="8">
         <v>0.57847222222222217</v>
       </c>
       <c r="D32">
@@ -4699,7 +4974,7 @@
       <c r="B33">
         <v>5</v>
       </c>
-      <c r="C33" s="30">
+      <c r="C33" s="22">
         <v>0.58124999999999993</v>
       </c>
       <c r="D33">
@@ -4740,7 +5015,7 @@
       <c r="B34">
         <v>3</v>
       </c>
-      <c r="C34" s="30">
+      <c r="C34" s="22">
         <v>0.59027777777777779</v>
       </c>
       <c r="D34">
@@ -4781,7 +5056,7 @@
       <c r="B35">
         <v>5</v>
       </c>
-      <c r="C35" s="30">
+      <c r="C35" s="8">
         <v>0.59305555555555556</v>
       </c>
       <c r="D35">
@@ -4822,7 +5097,7 @@
       <c r="B36">
         <v>3</v>
       </c>
-      <c r="C36" s="30">
+      <c r="C36" s="22">
         <v>0.6020833333333333</v>
       </c>
       <c r="D36">
@@ -4863,7 +5138,7 @@
       <c r="B37">
         <v>5</v>
       </c>
-      <c r="C37" s="30">
+      <c r="C37" s="22">
         <v>0.60416666666666663</v>
       </c>
       <c r="D37">
@@ -4904,7 +5179,7 @@
       <c r="B38">
         <v>3</v>
       </c>
-      <c r="C38" s="30">
+      <c r="C38" s="22">
         <v>0.6166666666666667</v>
       </c>
       <c r="D38">
@@ -4945,7 +5220,7 @@
       <c r="B39">
         <v>5</v>
       </c>
-      <c r="C39" s="30">
+      <c r="C39" s="22">
         <v>0.61875000000000002</v>
       </c>
       <c r="D39">
@@ -4978,13 +5253,9 @@
       <c r="M39" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="C40" s="30"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Code and data updates
</commit_message>
<xml_diff>
--- a/data/Bi-weekly_Tank_Sampling_2023.xlsx
+++ b/data/Bi-weekly_Tank_Sampling_2023.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl-my.sharepoint.com/personal/finnegan_roach_pnnl_gov/Documents/Documents/GitHub/mcdr_mesocosm_sensors/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\2023\Eelgrass_Mesocosm\Data_Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{0C670ED8-D985-4B58-A91B-EE790C36B6D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B580D81-93C3-4DA0-8757-8572E44E9419}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1AD106E-C0E2-42B7-A533-16B786E49401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="770" yWindow="0" windowWidth="18040" windowHeight="9510" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1160" yWindow="690" windowWidth="18040" windowHeight="9510" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="META" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="94">
   <si>
     <t xml:space="preserve">Tank T (C) </t>
   </si>
@@ -280,6 +280,48 @@
   <si>
     <t>J0.004756</t>
   </si>
+  <si>
+    <t>KP, FR</t>
+  </si>
+  <si>
+    <t>Switching to weekly c-sense maintenance, keeping biweekly for exos</t>
+  </si>
+  <si>
+    <t>Pulled for calibration</t>
+  </si>
+  <si>
+    <t>Putting exos back in post calibration, ended up pulling csense for a bit to make this easier</t>
+  </si>
+  <si>
+    <t>Had to recalibrate salinity on both exos and switch the salinity sensor on the bare exo</t>
+  </si>
+  <si>
+    <t>FR, NW</t>
+  </si>
+  <si>
+    <t>Installing pumped heads and pumps</t>
+  </si>
+  <si>
+    <t>Fixing flow through pumped heads, looked too low, changed fittings on pipework</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t>Increasing csense flow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New cal method for c-sense, pump cal gas through pumped heads instead of using bag </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Was working on code, accidentally didn’t record data </t>
+  </si>
+  <si>
+    <t>Flow got too low to measure any more samples, fix flow meter next time</t>
+  </si>
+  <si>
+    <t>Maybe forgot to shake up bottle for original point taken, so deleted and retook (that’s why time is later)</t>
+  </si>
 </sst>
 </file>
 
@@ -291,7 +333,7 @@
     <numFmt numFmtId="166" formatCode="h:mm:ss;@"/>
     <numFmt numFmtId="167" formatCode="[$-409]h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -317,6 +359,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -351,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -429,6 +478,10 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -772,9 +825,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CB21E28-2209-458E-B639-7E39D56BC310}">
   <dimension ref="A1:P134"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C92" sqref="C92"/>
+    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M130" sqref="M130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4508,183 +4561,999 @@
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A99" s="16">
+        <v>45138</v>
+      </c>
       <c r="B99" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="C99" s="19">
+        <v>0.49027777777777781</v>
+      </c>
+      <c r="D99">
+        <v>491.4</v>
+      </c>
+      <c r="E99">
+        <v>0.55820000000000003</v>
+      </c>
+      <c r="F99">
+        <v>0.61939999999999995</v>
+      </c>
+      <c r="G99">
+        <v>5.0410000000000003E-3</v>
+      </c>
+      <c r="H99">
+        <v>7.8979999999999997</v>
+      </c>
+      <c r="I99">
+        <v>1.342E-2</v>
+      </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A100" s="16">
+        <v>45138</v>
+      </c>
       <c r="B100" s="3">
         <v>1</v>
       </c>
+      <c r="C100" s="19">
+        <v>0.52361111111111114</v>
+      </c>
+      <c r="D100">
+        <v>413.5</v>
+      </c>
+      <c r="E100">
+        <v>0.58140000000000003</v>
+      </c>
+      <c r="F100">
+        <v>0.4909</v>
+      </c>
+      <c r="G100">
+        <v>1.5350000000000001E-2</v>
+      </c>
+      <c r="H100">
+        <v>5.4279999999999999</v>
+      </c>
+      <c r="I100">
+        <v>0.29039999999999999</v>
+      </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A101" s="16">
+        <v>45138</v>
+      </c>
       <c r="B101" s="3">
         <v>2</v>
       </c>
+      <c r="C101" s="19">
+        <v>0.52013888888888882</v>
+      </c>
+      <c r="D101">
+        <v>498.7</v>
+      </c>
+      <c r="E101">
+        <v>0.36509999999999998</v>
+      </c>
+      <c r="F101">
+        <v>0.52829999999999999</v>
+      </c>
+      <c r="G101">
+        <v>4.4470000000000004E-3</v>
+      </c>
+      <c r="H101">
+        <v>7.657</v>
+      </c>
+      <c r="I101">
+        <v>1.7559999999999999E-2</v>
+      </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A102" s="16">
+        <v>45138</v>
+      </c>
       <c r="B102" s="3">
         <v>3</v>
       </c>
+      <c r="C102" s="19">
+        <v>0.51597222222222217</v>
+      </c>
+      <c r="D102">
+        <v>497.5</v>
+      </c>
+      <c r="E102">
+        <v>0.51170000000000004</v>
+      </c>
+      <c r="F102">
+        <v>0.49619999999999997</v>
+      </c>
+      <c r="G102">
+        <v>5.2370000000000003E-3</v>
+      </c>
+      <c r="H102">
+        <v>6.2080000000000002</v>
+      </c>
+      <c r="I102">
+        <v>8.6899999999999998E-3</v>
+      </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A103" s="16">
+        <v>45138</v>
+      </c>
       <c r="B103" s="3">
         <v>4</v>
       </c>
+      <c r="C103" s="19">
+        <v>0.51180555555555551</v>
+      </c>
+      <c r="D103">
+        <v>431.2</v>
+      </c>
+      <c r="E103">
+        <v>0.55420000000000003</v>
+      </c>
+      <c r="F103">
+        <v>0.53680000000000005</v>
+      </c>
+      <c r="G103">
+        <v>3.7499999999999999E-3</v>
+      </c>
+      <c r="H103">
+        <v>8.6120000000000001</v>
+      </c>
+      <c r="I103">
+        <v>6.3540000000000003E-3</v>
+      </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A104" s="16">
+        <v>45138</v>
+      </c>
       <c r="B104" s="3">
         <v>5</v>
       </c>
+      <c r="C104" s="19">
+        <v>0.5083333333333333</v>
+      </c>
+      <c r="D104">
+        <v>622.4</v>
+      </c>
+      <c r="E104">
+        <v>0.94899999999999995</v>
+      </c>
+      <c r="F104">
+        <v>0.5393</v>
+      </c>
+      <c r="G104">
+        <v>4.6449999999999998E-3</v>
+      </c>
+      <c r="H104">
+        <v>7.0629999999999997</v>
+      </c>
+      <c r="I104">
+        <v>4.9659999999999999E-3</v>
+      </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A105" s="16">
+        <v>45138</v>
+      </c>
       <c r="B105" s="3">
         <v>6</v>
       </c>
+      <c r="C105" s="19">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="D105">
+        <v>478.7</v>
+      </c>
+      <c r="E105">
+        <v>0.88690000000000002</v>
+      </c>
+      <c r="F105">
+        <v>0.51339999999999997</v>
+      </c>
+      <c r="G105">
+        <v>4.9509999999999997E-3</v>
+      </c>
+      <c r="H105">
+        <v>6.3019999999999996</v>
+      </c>
+      <c r="I105">
+        <v>1.217E-3</v>
+      </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A106" s="16">
+        <v>45138</v>
+      </c>
       <c r="B106" s="3">
         <v>7</v>
       </c>
+      <c r="C106" s="19">
+        <v>0.4993055555555555</v>
+      </c>
+      <c r="D106">
+        <v>620.4</v>
+      </c>
+      <c r="E106">
+        <v>0.85560000000000003</v>
+      </c>
+      <c r="F106">
+        <v>0.5383</v>
+      </c>
+      <c r="G106">
+        <v>5.2620000000000002E-3</v>
+      </c>
+      <c r="H106">
+        <v>7.391</v>
+      </c>
+      <c r="I106">
+        <v>8.319E-3</v>
+      </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A107" s="16">
+        <v>45138</v>
+      </c>
       <c r="B107" s="3">
         <v>8</v>
       </c>
+      <c r="C107" s="19">
+        <v>0.49374999999999997</v>
+      </c>
+      <c r="D107">
+        <v>547.79999999999995</v>
+      </c>
+      <c r="E107">
+        <v>0.96399999999999997</v>
+      </c>
+      <c r="F107">
+        <v>0.52910000000000001</v>
+      </c>
+      <c r="G107">
+        <v>4.594E-3</v>
+      </c>
+      <c r="H107">
+        <v>7.335</v>
+      </c>
+      <c r="I107">
+        <v>4.1840000000000002E-3</v>
+      </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A108" s="16">
+        <v>45138</v>
+      </c>
       <c r="B108" s="3" t="s">
         <v>67</v>
       </c>
+      <c r="D108" s="32">
+        <v>408.7</v>
+      </c>
+      <c r="E108" s="32">
+        <v>0.60199999999999998</v>
+      </c>
+      <c r="F108" s="32">
+        <v>4.9889999999999997E-2</v>
+      </c>
+      <c r="G108" s="32">
+        <v>4.9630000000000004E-3</v>
+      </c>
+      <c r="H108" s="32">
+        <v>0.1099</v>
+      </c>
+      <c r="I108" s="32">
+        <v>6.7690000000000003E-4</v>
+      </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A109" s="16">
+        <v>45138</v>
+      </c>
       <c r="B109" s="3" t="s">
         <v>62</v>
       </c>
+      <c r="D109">
+        <v>410.4</v>
+      </c>
+      <c r="E109">
+        <v>0.4677</v>
+      </c>
+      <c r="F109">
+        <v>4.555E-2</v>
+      </c>
+      <c r="G109">
+        <v>5.3579999999999999E-3</v>
+      </c>
+      <c r="H109">
+        <v>0.10349999999999999</v>
+      </c>
+      <c r="I109">
+        <v>1.3359999999999999E-3</v>
+      </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A110" s="16">
+        <v>45138</v>
+      </c>
       <c r="B110" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="C110" s="19">
+        <v>0.49027777777777781</v>
+      </c>
+      <c r="D110">
+        <v>408.9</v>
+      </c>
+      <c r="E110">
+        <v>0.64319999999999999</v>
+      </c>
+      <c r="F110">
+        <v>0.36199999999999999</v>
+      </c>
+      <c r="G110">
+        <v>4.5690000000000001E-3</v>
+      </c>
+      <c r="H110">
+        <v>2.0649999999999999</v>
+      </c>
+      <c r="I110">
+        <v>7.7200000000000001E-4</v>
+      </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A111" s="16">
+        <v>45142</v>
+      </c>
       <c r="B111" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="C111" s="19">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="D111">
+        <v>562.20000000000005</v>
+      </c>
+      <c r="E111">
+        <v>1.3680000000000001</v>
+      </c>
+      <c r="F111">
+        <v>0.67269999999999996</v>
+      </c>
+      <c r="G111">
+        <v>5.2269999999999999E-3</v>
+      </c>
+      <c r="H111">
+        <v>7.4109999999999996</v>
+      </c>
+      <c r="I111">
+        <v>1.01E-2</v>
+      </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A112" s="16">
+        <v>45142</v>
+      </c>
       <c r="B112" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C112" s="19">
+        <v>0.62708333333333333</v>
+      </c>
+      <c r="D112">
+        <v>367.6</v>
+      </c>
+      <c r="E112">
+        <v>5.4980000000000002</v>
+      </c>
+      <c r="F112">
+        <v>0.46350000000000002</v>
+      </c>
+      <c r="G112">
+        <v>2.3089999999999999E-2</v>
+      </c>
+      <c r="H112">
+        <v>4.8879999999999999</v>
+      </c>
+      <c r="I112">
+        <v>0.53049999999999997</v>
+      </c>
+    </row>
+    <row r="113" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A113" s="16">
+        <v>45142</v>
+      </c>
       <c r="B113" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C113" s="19">
+        <v>0.62222222222222223</v>
+      </c>
+      <c r="D113">
+        <v>375.5</v>
+      </c>
+      <c r="E113">
+        <v>1.925</v>
+      </c>
+      <c r="F113">
+        <v>0.60450000000000004</v>
+      </c>
+      <c r="G113">
+        <v>1.0120000000000001E-2</v>
+      </c>
+      <c r="H113">
+        <v>8.2949999999999999</v>
+      </c>
+      <c r="I113">
+        <v>6.7180000000000004E-2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A114" s="16">
+        <v>45142</v>
+      </c>
       <c r="B114" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C114" s="19">
+        <v>0.61805555555555558</v>
+      </c>
+      <c r="D114">
+        <v>356.7</v>
+      </c>
+      <c r="E114">
+        <v>1.115</v>
+      </c>
+      <c r="F114">
+        <v>0.58360000000000001</v>
+      </c>
+      <c r="G114">
+        <v>4.0119999999999999E-3</v>
+      </c>
+      <c r="H114">
+        <v>8.2360000000000007</v>
+      </c>
+      <c r="I114">
+        <v>1.6789999999999999E-2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A115" s="16">
+        <v>45142</v>
+      </c>
       <c r="B115" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C115" s="19">
+        <v>0.61249999999999993</v>
+      </c>
+      <c r="D115">
+        <v>288.2</v>
+      </c>
+      <c r="E115">
+        <v>0.66930000000000001</v>
+      </c>
+      <c r="F115">
+        <v>0.59040000000000004</v>
+      </c>
+      <c r="G115">
+        <v>6.77E-3</v>
+      </c>
+      <c r="H115">
+        <v>9.2799999999999994</v>
+      </c>
+      <c r="I115">
+        <v>0.1119</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A116" s="16">
+        <v>45142</v>
+      </c>
       <c r="B116" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C116" s="19">
+        <v>0.60902777777777783</v>
+      </c>
+      <c r="D116">
+        <v>446.4</v>
+      </c>
+      <c r="E116">
+        <v>1.845</v>
+      </c>
+      <c r="F116">
+        <v>0.60770000000000002</v>
+      </c>
+      <c r="G116">
+        <v>4.8019999999999998E-3</v>
+      </c>
+      <c r="H116">
+        <v>8.9359999999999999</v>
+      </c>
+      <c r="I116">
+        <v>2.8719999999999999E-2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A117" s="16">
+        <v>45142</v>
+      </c>
       <c r="B117" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C117" s="19">
+        <v>0.60347222222222219</v>
+      </c>
+      <c r="D117">
+        <v>342.3</v>
+      </c>
+      <c r="E117">
+        <v>2.2679999999999998</v>
+      </c>
+      <c r="F117">
+        <v>0.59279999999999999</v>
+      </c>
+      <c r="G117">
+        <v>7.744E-3</v>
+      </c>
+      <c r="H117">
+        <v>8.11</v>
+      </c>
+      <c r="I117">
+        <v>1.8749999999999999E-2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A118" s="16">
+        <v>45142</v>
+      </c>
       <c r="B118" s="3">
         <v>7</v>
       </c>
-    </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C118" s="19">
+        <v>0.59930555555555554</v>
+      </c>
+      <c r="D118">
+        <v>509.6</v>
+      </c>
+      <c r="E118">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="F118">
+        <v>0.60329999999999995</v>
+      </c>
+      <c r="G118">
+        <v>4.2440000000000004E-3</v>
+      </c>
+      <c r="H118">
+        <v>9.0079999999999991</v>
+      </c>
+      <c r="I118">
+        <v>1.4330000000000001E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A119" s="16">
+        <v>45142</v>
+      </c>
       <c r="B119" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C119" s="19">
+        <v>0.59444444444444444</v>
+      </c>
+      <c r="D119">
+        <v>410.8</v>
+      </c>
+      <c r="E119">
+        <v>2.0259999999999998</v>
+      </c>
+      <c r="F119">
+        <v>0.60250000000000004</v>
+      </c>
+      <c r="G119">
+        <v>6.0610000000000004E-3</v>
+      </c>
+      <c r="H119">
+        <v>9.19</v>
+      </c>
+      <c r="I119">
+        <v>2.0629999999999999E-2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A120" s="16">
+        <v>45142</v>
+      </c>
       <c r="B120" s="3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="D120">
+        <v>404</v>
+      </c>
+      <c r="E120">
+        <v>1.194</v>
+      </c>
+      <c r="F120">
+        <v>2.0830000000000001E-2</v>
+      </c>
+      <c r="G120">
+        <v>3.9179999999999996E-3</v>
+      </c>
+      <c r="H120">
+        <v>4.5439999999999996</v>
+      </c>
+      <c r="I120">
+        <v>1.584E-2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A121" s="16">
+        <v>45142</v>
+      </c>
       <c r="B121" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="D121">
+        <v>392.9</v>
+      </c>
+      <c r="E121">
+        <v>0.55730000000000002</v>
+      </c>
+      <c r="F121">
+        <v>3.2190000000000003E-2</v>
+      </c>
+      <c r="G121">
+        <v>4.0470000000000002E-3</v>
+      </c>
+      <c r="H121">
+        <v>4.4589999999999996</v>
+      </c>
+      <c r="I121">
+        <v>2.4070000000000001E-2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A122" s="16">
+        <v>45142</v>
+      </c>
       <c r="B122" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C122" s="19">
+        <v>0.5854166666666667</v>
+      </c>
+      <c r="D122">
+        <v>409.4</v>
+      </c>
+      <c r="E122">
+        <v>0.41289999999999999</v>
+      </c>
+      <c r="F122">
+        <v>0.36149999999999999</v>
+      </c>
+      <c r="G122">
+        <v>5.0870000000000004E-3</v>
+      </c>
+      <c r="H122">
+        <v>2.0470000000000002</v>
+      </c>
+      <c r="I122">
+        <v>1.14E-3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A123" s="16">
+        <v>45152</v>
+      </c>
       <c r="B123" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C123" s="19">
+        <v>0.45694444444444443</v>
+      </c>
+      <c r="N123" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="124" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A124" s="16">
+        <v>45152</v>
+      </c>
       <c r="B124" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C124" s="19">
+        <v>0.49513888888888885</v>
+      </c>
+      <c r="D124">
+        <v>383.9</v>
+      </c>
+      <c r="E124">
+        <v>0.88929999999999998</v>
+      </c>
+      <c r="F124">
+        <v>0.63100000000000001</v>
+      </c>
+      <c r="G124">
+        <v>5.3270000000000001E-3</v>
+      </c>
+      <c r="H124">
+        <v>10.4</v>
+      </c>
+      <c r="I124">
+        <v>4.045E-3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A125" s="16">
+        <v>45152</v>
+      </c>
       <c r="B125" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C125" s="19">
+        <v>0.4909722222222222</v>
+      </c>
+      <c r="D125">
+        <v>498.8</v>
+      </c>
+      <c r="E125">
+        <v>1.39</v>
+      </c>
+      <c r="F125">
+        <v>0.58509999999999995</v>
+      </c>
+      <c r="G125">
+        <v>4.529E-3</v>
+      </c>
+      <c r="H125">
+        <v>8.9529999999999994</v>
+      </c>
+      <c r="I125">
+        <v>6.9769999999999997E-3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A126" s="16">
+        <v>45152</v>
+      </c>
       <c r="B126" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C126" s="19">
+        <v>0.48749999999999999</v>
+      </c>
+      <c r="D126">
+        <v>468.1</v>
+      </c>
+      <c r="E126">
+        <v>1.1990000000000001</v>
+      </c>
+      <c r="F126">
+        <v>0.61250000000000004</v>
+      </c>
+      <c r="G126">
+        <v>4.2119999999999996E-3</v>
+      </c>
+      <c r="H126">
+        <v>9.4819999999999993</v>
+      </c>
+      <c r="I126">
+        <v>4.7600000000000003E-3</v>
+      </c>
+    </row>
+    <row r="127" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A127" s="16">
+        <v>45152</v>
+      </c>
       <c r="B127" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C127" s="19">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="D127">
+        <v>418.1</v>
+      </c>
+      <c r="E127">
+        <v>1.365</v>
+      </c>
+      <c r="F127">
+        <v>0.61319999999999997</v>
+      </c>
+      <c r="G127">
+        <v>3.6080000000000001E-3</v>
+      </c>
+      <c r="H127">
+        <v>10.01</v>
+      </c>
+      <c r="I127">
+        <v>3.594E-3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A128" s="16">
+        <v>45152</v>
+      </c>
       <c r="B128" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C128" s="19">
+        <v>0.47638888888888892</v>
+      </c>
+      <c r="D128">
+        <v>520.5</v>
+      </c>
+      <c r="E128">
+        <v>1.8320000000000001</v>
+      </c>
+      <c r="F128">
+        <v>0.64349999999999996</v>
+      </c>
+      <c r="G128">
+        <v>4.0759999999999998E-3</v>
+      </c>
+      <c r="H128">
+        <v>9.2370000000000001</v>
+      </c>
+      <c r="I128">
+        <v>1.153E-2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A129" s="16">
+        <v>45152</v>
+      </c>
       <c r="B129" s="3">
         <v>6</v>
       </c>
-    </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C129" s="19">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="D129">
+        <v>480.6</v>
+      </c>
+      <c r="E129">
+        <v>0.41510000000000002</v>
+      </c>
+      <c r="F129">
+        <v>0.58430000000000004</v>
+      </c>
+      <c r="G129">
+        <v>5.1910000000000003E-3</v>
+      </c>
+      <c r="H129">
+        <v>8.8940000000000001</v>
+      </c>
+      <c r="I129">
+        <v>2.7130000000000001E-3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A130" s="16">
+        <v>45152</v>
+      </c>
       <c r="B130" s="3">
         <v>7</v>
       </c>
-    </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C130" s="19">
+        <v>0.4680555555555555</v>
+      </c>
+      <c r="D130">
+        <v>521.4</v>
+      </c>
+      <c r="E130">
+        <v>1.304</v>
+      </c>
+      <c r="F130">
+        <v>0.63549999999999995</v>
+      </c>
+      <c r="G130">
+        <v>4.3350000000000003E-3</v>
+      </c>
+      <c r="H130">
+        <v>10.28</v>
+      </c>
+      <c r="I130">
+        <v>3.1670000000000001E-3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A131" s="16">
+        <v>45152</v>
+      </c>
       <c r="B131" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C131" s="19">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="D131">
+        <v>467.7</v>
+      </c>
+      <c r="E131">
+        <v>1.9139999999999999</v>
+      </c>
+      <c r="F131">
+        <v>0.60570000000000002</v>
+      </c>
+      <c r="G131">
+        <v>6.8970000000000004E-3</v>
+      </c>
+      <c r="H131">
+        <v>9.6509999999999998</v>
+      </c>
+      <c r="I131">
+        <v>1.3679999999999999E-2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A132" s="16">
+        <v>45152</v>
+      </c>
       <c r="B132" s="3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="D132">
+        <v>397.8</v>
+      </c>
+      <c r="E132">
+        <v>0.34970000000000001</v>
+      </c>
+      <c r="F132">
+        <v>2.3290000000000002E-2</v>
+      </c>
+      <c r="G132">
+        <v>5.8919999999999997E-3</v>
+      </c>
+      <c r="H132">
+        <v>4.6059999999999999</v>
+      </c>
+      <c r="I132">
+        <v>9.567E-4</v>
+      </c>
+    </row>
+    <row r="133" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A133" s="16">
+        <v>45152</v>
+      </c>
       <c r="B133" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="N133" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="134" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A134" s="16">
+        <v>45152</v>
+      </c>
       <c r="B134" s="3" t="s">
         <v>31</v>
+      </c>
+      <c r="C134" s="19">
+        <v>0.4604166666666667</v>
+      </c>
+      <c r="D134">
+        <v>467.2</v>
+      </c>
+      <c r="E134">
+        <v>2.2069999999999999</v>
+      </c>
+      <c r="F134">
+        <v>0.36599999999999999</v>
+      </c>
+      <c r="G134">
+        <v>5.3030000000000004E-3</v>
+      </c>
+      <c r="H134">
+        <v>2.0190000000000001</v>
+      </c>
+      <c r="I134">
+        <v>1.3860000000000001E-3</v>
       </c>
     </row>
   </sheetData>
@@ -4696,10 +5565,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDFE220D-A5A4-4E15-86BE-B8CD9DC9EF8F}">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4727,7 +5596,7 @@
       <c r="C1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="33" t="s">
         <v>19</v>
       </c>
       <c r="E1" s="7" t="s">
@@ -4987,7 +5856,7 @@
       <c r="C8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="22">
+      <c r="D8" s="26">
         <v>0.4201388888888889</v>
       </c>
       <c r="E8" s="8">
@@ -5016,13 +5885,16 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>230711</v>
+      </c>
       <c r="B9" s="3">
         <v>5</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D9" s="26">
         <v>0.41805555555555557</v>
       </c>
       <c r="E9" s="8">
@@ -5051,58 +5923,481 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>230717</v>
+      </c>
       <c r="B10" s="3">
         <v>3</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="22"/>
+      <c r="C10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26">
+        <v>0.41388888888888892</v>
+      </c>
+      <c r="G10" s="8">
+        <v>0.42083333333333334</v>
+      </c>
+      <c r="H10" s="8">
+        <v>0.42986111111111108</v>
+      </c>
+      <c r="J10" s="8">
+        <v>0.44722222222222219</v>
+      </c>
+      <c r="K10" t="s">
+        <v>80</v>
+      </c>
+      <c r="L10" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>230717</v>
+      </c>
       <c r="B11" s="3">
         <v>5</v>
       </c>
-      <c r="D11" s="22"/>
+      <c r="C11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="26"/>
+      <c r="E11" s="8">
+        <v>0.41319444444444442</v>
+      </c>
+      <c r="G11" s="8">
+        <v>0.42083333333333334</v>
+      </c>
+      <c r="H11" s="8">
+        <v>0.42986111111111108</v>
+      </c>
+      <c r="J11" s="8">
+        <v>0.44861111111111113</v>
+      </c>
+      <c r="K11" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>230724</v>
+      </c>
       <c r="B12" s="3">
         <v>3</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="22"/>
+      <c r="C12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="26">
+        <v>0.60277777777777775</v>
+      </c>
+      <c r="K12" t="s">
+        <v>80</v>
+      </c>
+      <c r="L12" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>230724</v>
+      </c>
       <c r="B13" s="3">
         <v>5</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="22"/>
+      <c r="C13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="26">
+        <v>0.60069444444444442</v>
+      </c>
+      <c r="K13" t="s">
+        <v>80</v>
+      </c>
+      <c r="L13" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>230725</v>
+      </c>
       <c r="B14" s="3">
         <v>3</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="22"/>
+      <c r="C14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="26"/>
+      <c r="E14" s="8">
+        <v>0.45208333333333334</v>
+      </c>
+      <c r="G14" s="8">
+        <v>0.46111111111111108</v>
+      </c>
+      <c r="H14" s="8">
+        <v>0.46875</v>
+      </c>
+      <c r="J14" s="8">
+        <v>0.47986111111111113</v>
+      </c>
+      <c r="K14" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>230725</v>
+      </c>
       <c r="B15" s="3">
         <v>5</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="22"/>
+      <c r="C15" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="26"/>
+      <c r="E15" s="8">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="G15" s="8">
+        <v>0.46111111111111108</v>
+      </c>
+      <c r="H15" s="8">
+        <v>0.46875</v>
+      </c>
+      <c r="J15" s="8">
+        <v>0.47847222222222219</v>
+      </c>
+      <c r="K15" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>230726</v>
+      </c>
       <c r="B16" s="3">
         <v>3</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="22"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="C16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="26"/>
+      <c r="E16" s="8">
+        <v>0.50694444444444442</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="I16" s="8">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="J16" s="8">
+        <v>0.50902777777777775</v>
+      </c>
+      <c r="K16" t="s">
+        <v>80</v>
+      </c>
+      <c r="L16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>230726</v>
+      </c>
       <c r="B17" s="3">
         <v>5</v>
       </c>
+      <c r="C17" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="D17" s="22"/>
+      <c r="E17" s="8">
+        <v>0.50486111111111109</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="I17" s="8">
+        <v>0.50694444444444442</v>
+      </c>
+      <c r="J17" s="8">
+        <v>0.50694444444444442</v>
+      </c>
+      <c r="K17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>230728</v>
+      </c>
+      <c r="B18" s="3">
+        <v>3</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="8">
+        <v>0.35555555555555557</v>
+      </c>
+      <c r="F18" s="8">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="I18" s="8">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="K18" t="s">
+        <v>80</v>
+      </c>
+      <c r="L18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>230728</v>
+      </c>
+      <c r="B19" s="3">
+        <v>5</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="8">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="F19" s="8">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="I19" s="8">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="K19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>230801</v>
+      </c>
+      <c r="B20" s="3">
+        <v>3</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8">
+        <v>0.54305555555555551</v>
+      </c>
+      <c r="G20" s="8">
+        <v>0.55763888888888891</v>
+      </c>
+      <c r="H20" s="8">
+        <v>0.56597222222222221</v>
+      </c>
+      <c r="J20" s="8">
+        <v>0.625</v>
+      </c>
+      <c r="K20" t="s">
+        <v>85</v>
+      </c>
+      <c r="L20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>230801</v>
+      </c>
+      <c r="B21" s="3">
+        <v>5</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8">
+        <v>0.54375000000000007</v>
+      </c>
+      <c r="G21" s="8">
+        <v>0.55763888888888891</v>
+      </c>
+      <c r="H21" s="8">
+        <v>0.56597222222222221</v>
+      </c>
+      <c r="J21" s="8">
+        <v>0.63402777777777775</v>
+      </c>
+      <c r="K21" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>230802</v>
+      </c>
+      <c r="B22" s="3">
+        <v>3</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8">
+        <v>0.44930555555555557</v>
+      </c>
+      <c r="J22" s="8">
+        <v>0.4548611111111111</v>
+      </c>
+      <c r="K22" t="s">
+        <v>88</v>
+      </c>
+      <c r="L22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>230802</v>
+      </c>
+      <c r="B23" s="3">
+        <v>5</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8">
+        <v>0.43194444444444446</v>
+      </c>
+      <c r="J23" s="8">
+        <v>0.44930555555555557</v>
+      </c>
+      <c r="K23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>230804</v>
+      </c>
+      <c r="B24" s="3">
+        <v>5</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="8">
+        <v>0.38958333333333334</v>
+      </c>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8">
+        <v>0.40138888888888885</v>
+      </c>
+      <c r="K24" t="s">
+        <v>88</v>
+      </c>
+      <c r="L24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>230804</v>
+      </c>
+      <c r="B25" s="3">
+        <v>3</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="8">
+        <v>0.40138888888888885</v>
+      </c>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8">
+        <v>0.4055555555555555</v>
+      </c>
+      <c r="K25" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>230807</v>
+      </c>
+      <c r="B26" s="3">
+        <v>3</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="8">
+        <v>0.60972222222222217</v>
+      </c>
+      <c r="E26" s="8">
+        <v>0.60972222222222217</v>
+      </c>
+      <c r="F26" s="8">
+        <v>0.63055555555555554</v>
+      </c>
+      <c r="G26" s="8">
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="H26" s="8">
+        <v>0.67013888888888884</v>
+      </c>
+      <c r="I26" s="8">
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="J26" s="8">
+        <v>0.68958333333333333</v>
+      </c>
+      <c r="K26" t="s">
+        <v>88</v>
+      </c>
+      <c r="L26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>230807</v>
+      </c>
+      <c r="B27" s="3">
+        <v>5</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="8">
+        <v>0.6118055555555556</v>
+      </c>
+      <c r="E27" s="8">
+        <v>0.6118055555555556</v>
+      </c>
+      <c r="F27" s="8">
+        <v>0.63055555555555554</v>
+      </c>
+      <c r="G27" s="8">
+        <v>0.64236111111111105</v>
+      </c>
+      <c r="H27" s="8">
+        <v>0.66041666666666665</v>
+      </c>
+      <c r="I27" s="8">
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="J27" s="8">
+        <v>0.68680555555555556</v>
+      </c>
+      <c r="K27" t="s">
+        <v>88</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5112,10 +6407,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{219CC811-8442-4429-81C5-6ADB9C52A9AC}">
-  <dimension ref="A1:N74"/>
+  <dimension ref="A1:N92"/>
   <sheetViews>
-    <sheetView topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7695,6 +8990,531 @@
         <v>7.4739999999999995E-4</v>
       </c>
     </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A75" s="16">
+        <v>45154</v>
+      </c>
+      <c r="B75" t="s">
+        <v>78</v>
+      </c>
+      <c r="C75" s="22">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="D75">
+        <v>400.2</v>
+      </c>
+      <c r="E75">
+        <v>1.694</v>
+      </c>
+      <c r="F75">
+        <v>1.486E-2</v>
+      </c>
+      <c r="G75">
+        <v>5.9760000000000004E-3</v>
+      </c>
+      <c r="H75">
+        <v>4.5759999999999996</v>
+      </c>
+      <c r="I75">
+        <v>9.9649999999999999E-3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A76" s="16">
+        <v>45154</v>
+      </c>
+      <c r="B76">
+        <v>5</v>
+      </c>
+      <c r="C76" s="22">
+        <v>0.34166666666666662</v>
+      </c>
+      <c r="D76">
+        <v>690.3</v>
+      </c>
+      <c r="E76">
+        <v>6.4459999999999997</v>
+      </c>
+      <c r="F76">
+        <v>0.65820000000000001</v>
+      </c>
+      <c r="G76">
+        <v>8.7550000000000006E-3</v>
+      </c>
+      <c r="H76">
+        <v>8.7560000000000002</v>
+      </c>
+      <c r="I76">
+        <v>6.1280000000000001E-2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A77" s="16">
+        <v>45154</v>
+      </c>
+      <c r="B77">
+        <v>3</v>
+      </c>
+      <c r="C77" s="22">
+        <v>0.35069444444444442</v>
+      </c>
+      <c r="D77">
+        <v>703.9</v>
+      </c>
+      <c r="E77">
+        <v>3.4140000000000001</v>
+      </c>
+      <c r="F77">
+        <v>0.58930000000000005</v>
+      </c>
+      <c r="G77">
+        <v>8.2579999999999997E-3</v>
+      </c>
+      <c r="H77">
+        <v>7.24</v>
+      </c>
+      <c r="I77">
+        <v>6.7089999999999997E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A78" s="16">
+        <v>45154</v>
+      </c>
+      <c r="B78">
+        <v>5</v>
+      </c>
+      <c r="C78" s="22">
+        <v>0.38055555555555554</v>
+      </c>
+      <c r="D78">
+        <v>630.20000000000005</v>
+      </c>
+      <c r="E78">
+        <v>0.7732</v>
+      </c>
+      <c r="F78">
+        <v>0.64710000000000001</v>
+      </c>
+      <c r="G78">
+        <v>6.6400000000000001E-3</v>
+      </c>
+      <c r="H78">
+        <v>8.9640000000000004</v>
+      </c>
+      <c r="I78">
+        <v>2.7400000000000001E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A79" s="16">
+        <v>45154</v>
+      </c>
+      <c r="B79">
+        <v>3</v>
+      </c>
+      <c r="C79" s="22">
+        <v>0.38750000000000001</v>
+      </c>
+      <c r="D79">
+        <v>700.3</v>
+      </c>
+      <c r="E79">
+        <v>1.877</v>
+      </c>
+      <c r="F79">
+        <v>0.65810000000000002</v>
+      </c>
+      <c r="G79">
+        <v>4.8300000000000001E-3</v>
+      </c>
+      <c r="H79">
+        <v>8.68</v>
+      </c>
+      <c r="I79">
+        <v>6.058E-3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A80" s="16">
+        <v>45154</v>
+      </c>
+      <c r="B80">
+        <v>5</v>
+      </c>
+      <c r="C80" s="22">
+        <v>0.4152777777777778</v>
+      </c>
+      <c r="D80">
+        <v>658</v>
+      </c>
+      <c r="E80">
+        <v>0.91769999999999996</v>
+      </c>
+      <c r="F80">
+        <v>0.67949999999999999</v>
+      </c>
+      <c r="G80">
+        <v>4.5659999999999997E-3</v>
+      </c>
+      <c r="H80">
+        <v>9.734</v>
+      </c>
+      <c r="I80">
+        <v>3.6180000000000001E-3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A81" s="16">
+        <v>45154</v>
+      </c>
+      <c r="B81">
+        <v>3</v>
+      </c>
+      <c r="C81" s="22">
+        <v>0.42083333333333334</v>
+      </c>
+      <c r="D81">
+        <v>673.1</v>
+      </c>
+      <c r="E81">
+        <v>1.0189999999999999</v>
+      </c>
+      <c r="F81">
+        <v>0.64070000000000005</v>
+      </c>
+      <c r="G81">
+        <v>4.8120000000000003E-3</v>
+      </c>
+      <c r="H81">
+        <v>8.4410000000000007</v>
+      </c>
+      <c r="I81">
+        <v>7.1139999999999997E-3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A82" s="16">
+        <v>45154</v>
+      </c>
+      <c r="B82">
+        <v>5</v>
+      </c>
+      <c r="C82" s="22">
+        <v>0.4604166666666667</v>
+      </c>
+      <c r="D82">
+        <v>626.5</v>
+      </c>
+      <c r="E82">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="F82">
+        <v>0.68799999999999994</v>
+      </c>
+      <c r="G82">
+        <v>4.3010000000000001E-3</v>
+      </c>
+      <c r="H82">
+        <v>9.6460000000000008</v>
+      </c>
+      <c r="I82">
+        <v>1.8069999999999999E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A83" s="16">
+        <v>45154</v>
+      </c>
+      <c r="B83">
+        <v>3</v>
+      </c>
+      <c r="C83" s="22">
+        <v>0.46736111111111112</v>
+      </c>
+      <c r="D83">
+        <v>584.6</v>
+      </c>
+      <c r="E83">
+        <v>0.6472</v>
+      </c>
+      <c r="F83">
+        <v>0.65239999999999998</v>
+      </c>
+      <c r="G83">
+        <v>3.5769999999999999E-3</v>
+      </c>
+      <c r="H83">
+        <v>8.7059999999999995</v>
+      </c>
+      <c r="I83">
+        <v>8.9499999999999996E-4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A84" s="16">
+        <v>45154</v>
+      </c>
+      <c r="B84">
+        <v>5</v>
+      </c>
+      <c r="C84" s="22">
+        <v>0.50277777777777777</v>
+      </c>
+      <c r="D84">
+        <v>546.4</v>
+      </c>
+      <c r="E84">
+        <v>3.19</v>
+      </c>
+      <c r="F84">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="G84">
+        <v>5.0559999999999997E-3</v>
+      </c>
+      <c r="H84">
+        <v>7.915</v>
+      </c>
+      <c r="I84">
+        <v>6.6949999999999996E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A85" s="16">
+        <v>45154</v>
+      </c>
+      <c r="B85">
+        <v>3</v>
+      </c>
+      <c r="C85" s="22">
+        <v>0.53611111111111109</v>
+      </c>
+      <c r="D85">
+        <v>471.9</v>
+      </c>
+      <c r="E85">
+        <v>1.2829999999999999</v>
+      </c>
+      <c r="F85">
+        <v>0.64</v>
+      </c>
+      <c r="G85">
+        <v>2.702E-3</v>
+      </c>
+      <c r="H85">
+        <v>8.3450000000000006</v>
+      </c>
+      <c r="I85">
+        <v>1.6469999999999999E-2</v>
+      </c>
+      <c r="N85" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A86" s="16">
+        <v>45154</v>
+      </c>
+      <c r="B86">
+        <v>5</v>
+      </c>
+      <c r="C86" s="22">
+        <v>0.54513888888888895</v>
+      </c>
+      <c r="D86">
+        <v>533.5</v>
+      </c>
+      <c r="E86">
+        <v>0.64390000000000003</v>
+      </c>
+      <c r="F86">
+        <v>0.69610000000000005</v>
+      </c>
+      <c r="G86">
+        <v>5.2209999999999999E-3</v>
+      </c>
+      <c r="H86">
+        <v>10.19</v>
+      </c>
+      <c r="I86">
+        <v>4.4730000000000004E-3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A87" s="16">
+        <v>45154</v>
+      </c>
+      <c r="B87">
+        <v>3</v>
+      </c>
+      <c r="C87" s="22">
+        <v>0.55138888888888882</v>
+      </c>
+      <c r="D87">
+        <v>443.4</v>
+      </c>
+      <c r="E87">
+        <v>0.78510000000000002</v>
+      </c>
+      <c r="F87">
+        <v>0.62780000000000002</v>
+      </c>
+      <c r="G87">
+        <v>4.797E-3</v>
+      </c>
+      <c r="H87">
+        <v>7.9320000000000004</v>
+      </c>
+      <c r="I87">
+        <v>5.7359999999999998E-3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A88" s="16">
+        <v>45154</v>
+      </c>
+      <c r="B88">
+        <v>5</v>
+      </c>
+      <c r="C88" s="22">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D88">
+        <v>503</v>
+      </c>
+      <c r="E88">
+        <v>0.8518</v>
+      </c>
+      <c r="F88">
+        <v>0.6946</v>
+      </c>
+      <c r="G88">
+        <v>3.447E-3</v>
+      </c>
+      <c r="H88">
+        <v>8.5809999999999995</v>
+      </c>
+      <c r="I88">
+        <v>1.7210000000000001E-3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A89" s="16">
+        <v>45154</v>
+      </c>
+      <c r="B89">
+        <v>3</v>
+      </c>
+      <c r="C89" s="22">
+        <v>0.58819444444444446</v>
+      </c>
+      <c r="D89">
+        <v>411.1</v>
+      </c>
+      <c r="E89">
+        <v>0.94089999999999996</v>
+      </c>
+      <c r="F89">
+        <v>0.65349999999999997</v>
+      </c>
+      <c r="G89">
+        <v>4.2649999999999997E-3</v>
+      </c>
+      <c r="H89">
+        <v>7.7329999999999997</v>
+      </c>
+      <c r="I89">
+        <v>3.4160000000000002E-3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A90" s="16">
+        <v>45154</v>
+      </c>
+      <c r="B90">
+        <v>5</v>
+      </c>
+      <c r="C90" s="22">
+        <v>0.62708333333333333</v>
+      </c>
+      <c r="D90">
+        <v>490.1</v>
+      </c>
+      <c r="E90">
+        <v>1.903</v>
+      </c>
+      <c r="F90">
+        <v>0.7046</v>
+      </c>
+      <c r="G90">
+        <v>3.7269999999999998E-3</v>
+      </c>
+      <c r="H90">
+        <v>8.7159999999999993</v>
+      </c>
+      <c r="I90">
+        <v>8.4639999999999993E-3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A91" s="16">
+        <v>45154</v>
+      </c>
+      <c r="B91">
+        <v>3</v>
+      </c>
+      <c r="C91" s="22">
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="D91">
+        <v>356</v>
+      </c>
+      <c r="E91">
+        <v>0.5605</v>
+      </c>
+      <c r="F91">
+        <v>0.63119999999999998</v>
+      </c>
+      <c r="G91">
+        <v>4.803E-3</v>
+      </c>
+      <c r="H91">
+        <v>6.6660000000000004</v>
+      </c>
+      <c r="I91">
+        <v>6.9690000000000004E-3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A92" s="16">
+        <v>45154</v>
+      </c>
+      <c r="B92" t="s">
+        <v>78</v>
+      </c>
+      <c r="C92" s="22">
+        <v>0.64444444444444449</v>
+      </c>
+      <c r="D92">
+        <v>408.8</v>
+      </c>
+      <c r="E92">
+        <v>0.25309999999999999</v>
+      </c>
+      <c r="F92">
+        <v>4.2079999999999999E-2</v>
+      </c>
+      <c r="G92">
+        <v>4.3610000000000003E-3</v>
+      </c>
+      <c r="H92">
+        <v>4.5570000000000004</v>
+      </c>
+      <c r="I92">
+        <v>1.408E-3</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updating scripts and datasets
</commit_message>
<xml_diff>
--- a/data/Bi-weekly_Tank_Sampling_2023.xlsx
+++ b/data/Bi-weekly_Tank_Sampling_2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\2023\Eelgrass_Mesocosm\Data_Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1AD106E-C0E2-42B7-A533-16B786E49401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD578CA0-9B9F-42E4-9E70-24A46D9FC2C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="690" windowWidth="18040" windowHeight="9510" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1070" yWindow="0" windowWidth="18040" windowHeight="9510" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="META" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="97">
   <si>
     <t xml:space="preserve">Tank T (C) </t>
   </si>
@@ -321,6 +321,15 @@
   </si>
   <si>
     <t>Maybe forgot to shake up bottle for original point taken, so deleted and retook (that’s why time is later)</t>
+  </si>
+  <si>
+    <t>(spent night in lab)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not doing csense cal check because cal gas is low and should develop better calibration protocol </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fixing csense flow, took off pumped head, cleaned membrane, changed one of the fittings with a smaller one </t>
   </si>
 </sst>
 </file>
@@ -823,11 +832,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CB21E28-2209-458E-B639-7E39D56BC310}">
-  <dimension ref="A1:P134"/>
+  <dimension ref="A1:P146"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M130" sqref="M130"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J145" sqref="J145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5556,6 +5565,348 @@
         <v>1.3860000000000001E-3</v>
       </c>
     </row>
+    <row r="135" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A135" s="16">
+        <v>45156</v>
+      </c>
+      <c r="B135" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C135" s="19">
+        <v>0.4291666666666667</v>
+      </c>
+      <c r="D135">
+        <v>590.20000000000005</v>
+      </c>
+      <c r="E135">
+        <v>1.4330000000000001</v>
+      </c>
+      <c r="F135">
+        <v>0.62280000000000002</v>
+      </c>
+      <c r="G135">
+        <v>4.2810000000000001E-3</v>
+      </c>
+      <c r="H135">
+        <v>10.8</v>
+      </c>
+      <c r="I135">
+        <v>4.1079999999999997E-3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A136" s="16">
+        <v>45156</v>
+      </c>
+      <c r="B136" s="3">
+        <v>1</v>
+      </c>
+      <c r="C136" s="19">
+        <v>0.45</v>
+      </c>
+      <c r="D136">
+        <v>549.6</v>
+      </c>
+      <c r="E136">
+        <v>0.58120000000000005</v>
+      </c>
+      <c r="F136">
+        <v>0.63849999999999996</v>
+      </c>
+      <c r="G136">
+        <v>4.5380000000000004E-3</v>
+      </c>
+      <c r="H136">
+        <v>5.8789999999999996</v>
+      </c>
+      <c r="I136">
+        <v>1.094E-2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A137" s="16">
+        <v>45156</v>
+      </c>
+      <c r="B137" s="3">
+        <v>2</v>
+      </c>
+      <c r="C137" s="19">
+        <v>0.44861111111111113</v>
+      </c>
+      <c r="D137">
+        <v>576.29999999999995</v>
+      </c>
+      <c r="E137">
+        <v>1.0529999999999999</v>
+      </c>
+      <c r="F137">
+        <v>0.59640000000000004</v>
+      </c>
+      <c r="G137">
+        <v>4.5360000000000001E-3</v>
+      </c>
+      <c r="H137">
+        <v>9.7070000000000007</v>
+      </c>
+      <c r="I137">
+        <v>1.089E-2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A138" s="16">
+        <v>45156</v>
+      </c>
+      <c r="B138" s="3">
+        <v>3</v>
+      </c>
+      <c r="C138" s="19">
+        <v>0.44305555555555554</v>
+      </c>
+      <c r="D138">
+        <v>631</v>
+      </c>
+      <c r="E138">
+        <v>1.008</v>
+      </c>
+      <c r="F138">
+        <v>0.59850000000000003</v>
+      </c>
+      <c r="G138">
+        <v>3.9199999999999999E-3</v>
+      </c>
+      <c r="H138">
+        <v>6.9870000000000001</v>
+      </c>
+      <c r="I138">
+        <v>5.5269999999999998E-3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A139" s="16">
+        <v>45156</v>
+      </c>
+      <c r="B139" s="3">
+        <v>4</v>
+      </c>
+      <c r="C139" s="19">
+        <v>0.44166666666666665</v>
+      </c>
+      <c r="D139">
+        <v>673.8</v>
+      </c>
+      <c r="E139">
+        <v>0.68979999999999997</v>
+      </c>
+      <c r="F139">
+        <v>0.6149</v>
+      </c>
+      <c r="G139">
+        <v>4.7080000000000004E-3</v>
+      </c>
+      <c r="H139">
+        <v>10.38</v>
+      </c>
+      <c r="I139">
+        <v>7.4609999999999998E-3</v>
+      </c>
+    </row>
+    <row r="140" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A140" s="16">
+        <v>45156</v>
+      </c>
+      <c r="B140" s="3">
+        <v>5</v>
+      </c>
+      <c r="C140" s="19">
+        <v>0.4381944444444445</v>
+      </c>
+      <c r="D140">
+        <v>642.9</v>
+      </c>
+      <c r="E140">
+        <v>0.85429999999999995</v>
+      </c>
+      <c r="F140">
+        <v>0.65559999999999996</v>
+      </c>
+      <c r="G140">
+        <v>5.5459999999999997E-3</v>
+      </c>
+      <c r="H140">
+        <v>8.2309999999999999</v>
+      </c>
+      <c r="I140">
+        <v>3.8670000000000002E-3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A141" s="16">
+        <v>45156</v>
+      </c>
+      <c r="B141" s="3">
+        <v>6</v>
+      </c>
+      <c r="C141" s="19">
+        <v>0.43541666666666662</v>
+      </c>
+      <c r="D141">
+        <v>648.1</v>
+      </c>
+      <c r="E141">
+        <v>1.6819999999999999</v>
+      </c>
+      <c r="F141">
+        <v>0.59430000000000005</v>
+      </c>
+      <c r="G141">
+        <v>3.8059999999999999E-3</v>
+      </c>
+      <c r="H141">
+        <v>9.0820000000000007</v>
+      </c>
+      <c r="I141">
+        <v>9.8239999999999994E-3</v>
+      </c>
+    </row>
+    <row r="142" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A142" s="16">
+        <v>45156</v>
+      </c>
+      <c r="B142" s="3">
+        <v>7</v>
+      </c>
+      <c r="C142" s="19">
+        <v>0.43263888888888885</v>
+      </c>
+      <c r="D142">
+        <v>658.4</v>
+      </c>
+      <c r="E142">
+        <v>1.579</v>
+      </c>
+      <c r="F142">
+        <v>0.62809999999999999</v>
+      </c>
+      <c r="G142">
+        <v>5.6870000000000002E-3</v>
+      </c>
+      <c r="H142">
+        <v>6.9050000000000002</v>
+      </c>
+      <c r="I142">
+        <v>1.8079999999999999E-2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A143" s="16">
+        <v>45156</v>
+      </c>
+      <c r="B143" s="3">
+        <v>8</v>
+      </c>
+      <c r="C143" s="19">
+        <v>0.4284722222222222</v>
+      </c>
+      <c r="D143">
+        <v>640</v>
+      </c>
+      <c r="E143">
+        <v>1.7330000000000001</v>
+      </c>
+      <c r="F143">
+        <v>0.59309999999999996</v>
+      </c>
+      <c r="G143">
+        <v>4.9150000000000001E-3</v>
+      </c>
+      <c r="H143">
+        <v>7.0540000000000003</v>
+      </c>
+      <c r="I143">
+        <v>1.703E-2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A144" s="16">
+        <v>45156</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D144">
+        <v>405.8</v>
+      </c>
+      <c r="E144">
+        <v>0.72040000000000004</v>
+      </c>
+      <c r="F144">
+        <v>1.9210000000000001E-2</v>
+      </c>
+      <c r="G144">
+        <v>5.1190000000000003E-3</v>
+      </c>
+      <c r="H144">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="I144">
+        <v>2.3649999999999999E-3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A145" s="16">
+        <v>45156</v>
+      </c>
+      <c r="B145" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D145">
+        <v>408.7</v>
+      </c>
+      <c r="E145">
+        <v>1.234</v>
+      </c>
+      <c r="F145">
+        <v>3.4270000000000002E-2</v>
+      </c>
+      <c r="G145">
+        <v>3.5279999999999999E-3</v>
+      </c>
+      <c r="H145">
+        <v>4.5140000000000002</v>
+      </c>
+      <c r="I145">
+        <v>8.5749999999999993E-3</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A146" s="16">
+        <v>45156</v>
+      </c>
+      <c r="B146" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C146" s="19">
+        <v>0.42777777777777781</v>
+      </c>
+      <c r="D146">
+        <v>418</v>
+      </c>
+      <c r="E146">
+        <v>0.51570000000000005</v>
+      </c>
+      <c r="F146">
+        <v>0.36049999999999999</v>
+      </c>
+      <c r="G146">
+        <v>5.4460000000000003E-3</v>
+      </c>
+      <c r="H146">
+        <v>2.0430000000000001</v>
+      </c>
+      <c r="I146">
+        <v>1.4499999999999999E-3</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5565,10 +5916,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDFE220D-A5A4-4E15-86BE-B8CD9DC9EF8F}">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5924,47 +6275,38 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>230717</v>
+        <v>230712</v>
       </c>
       <c r="B10" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26">
-        <v>0.41388888888888892</v>
-      </c>
-      <c r="G10" s="8">
-        <v>0.42083333333333334</v>
-      </c>
-      <c r="H10" s="8">
-        <v>0.42986111111111108</v>
-      </c>
-      <c r="J10" s="8">
-        <v>0.44722222222222219</v>
-      </c>
-      <c r="K10" t="s">
-        <v>80</v>
-      </c>
-      <c r="L10" t="s">
-        <v>81</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8">
+        <v>0.40625</v>
+      </c>
+      <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>230717</v>
       </c>
       <c r="B11" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="26"/>
-      <c r="E11" s="8">
-        <v>0.41319444444444442</v>
+      <c r="E11" s="26">
+        <v>0.41388888888888892</v>
       </c>
       <c r="G11" s="8">
         <v>0.42083333333333334</v>
@@ -5973,30 +6315,40 @@
         <v>0.42986111111111108</v>
       </c>
       <c r="J11" s="8">
-        <v>0.44861111111111113</v>
+        <v>0.44722222222222219</v>
       </c>
       <c r="K11" t="s">
         <v>80</v>
       </c>
+      <c r="L11" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>230724</v>
+        <v>230717</v>
       </c>
       <c r="B12" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="26">
-        <v>0.60277777777777775</v>
+        <v>14</v>
+      </c>
+      <c r="D12" s="26"/>
+      <c r="E12" s="8">
+        <v>0.41319444444444442</v>
+      </c>
+      <c r="G12" s="8">
+        <v>0.42083333333333334</v>
+      </c>
+      <c r="H12" s="8">
+        <v>0.42986111111111108</v>
+      </c>
+      <c r="J12" s="8">
+        <v>0.44861111111111113</v>
       </c>
       <c r="K12" t="s">
         <v>80</v>
-      </c>
-      <c r="L12" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
@@ -6004,13 +6356,13 @@
         <v>230724</v>
       </c>
       <c r="B13" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D13" s="26">
-        <v>0.60069444444444442</v>
+        <v>0.60277777777777775</v>
       </c>
       <c r="K13" t="s">
         <v>80</v>
@@ -6021,29 +6373,22 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>230725</v>
+        <v>230724</v>
       </c>
       <c r="B14" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="8">
-        <v>0.45208333333333334</v>
-      </c>
-      <c r="G14" s="8">
-        <v>0.46111111111111108</v>
-      </c>
-      <c r="H14" s="8">
-        <v>0.46875</v>
-      </c>
-      <c r="J14" s="8">
-        <v>0.47986111111111113</v>
+        <v>14</v>
+      </c>
+      <c r="D14" s="26">
+        <v>0.60069444444444442</v>
       </c>
       <c r="K14" t="s">
         <v>80</v>
+      </c>
+      <c r="L14" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
@@ -6051,14 +6396,14 @@
         <v>230725</v>
       </c>
       <c r="B15" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15" s="26"/>
       <c r="E15" s="8">
-        <v>0.4513888888888889</v>
+        <v>0.45208333333333334</v>
       </c>
       <c r="G15" s="8">
         <v>0.46111111111111108</v>
@@ -6067,7 +6412,7 @@
         <v>0.46875</v>
       </c>
       <c r="J15" s="8">
-        <v>0.47847222222222219</v>
+        <v>0.47986111111111113</v>
       </c>
       <c r="K15" t="s">
         <v>80</v>
@@ -6075,32 +6420,29 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>230726</v>
+        <v>230725</v>
       </c>
       <c r="B16" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D16" s="26"/>
       <c r="E16" s="8">
-        <v>0.50694444444444442</v>
-      </c>
-      <c r="F16" s="8">
-        <v>0.4826388888888889</v>
-      </c>
-      <c r="I16" s="8">
-        <v>0.51041666666666663</v>
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="G16" s="8">
+        <v>0.46111111111111108</v>
+      </c>
+      <c r="H16" s="8">
+        <v>0.46875</v>
       </c>
       <c r="J16" s="8">
-        <v>0.50902777777777775</v>
+        <v>0.47847222222222219</v>
       </c>
       <c r="K16" t="s">
         <v>80</v>
-      </c>
-      <c r="L16" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
@@ -6108,52 +6450,56 @@
         <v>230726</v>
       </c>
       <c r="B17" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="22"/>
+        <v>13</v>
+      </c>
+      <c r="D17" s="26"/>
       <c r="E17" s="8">
-        <v>0.50486111111111109</v>
+        <v>0.50694444444444442</v>
       </c>
       <c r="F17" s="8">
         <v>0.4826388888888889</v>
       </c>
       <c r="I17" s="8">
-        <v>0.50694444444444442</v>
+        <v>0.51041666666666663</v>
       </c>
       <c r="J17" s="8">
-        <v>0.50694444444444442</v>
+        <v>0.50902777777777775</v>
       </c>
       <c r="K17" t="s">
         <v>80</v>
       </c>
+      <c r="L17" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>230728</v>
+        <v>230726</v>
       </c>
       <c r="B18" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="8">
-        <v>0.35555555555555557</v>
+        <v>14</v>
+      </c>
+      <c r="D18" s="22"/>
+      <c r="E18" s="8">
+        <v>0.50486111111111109</v>
       </c>
       <c r="F18" s="8">
-        <v>0.45833333333333331</v>
+        <v>0.4826388888888889</v>
       </c>
       <c r="I18" s="8">
-        <v>0.4861111111111111</v>
+        <v>0.50694444444444442</v>
+      </c>
+      <c r="J18" s="8">
+        <v>0.50694444444444442</v>
       </c>
       <c r="K18" t="s">
         <v>80</v>
-      </c>
-      <c r="L18" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.35">
@@ -6161,13 +6507,13 @@
         <v>230728</v>
       </c>
       <c r="B19" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D19" s="8">
-        <v>0.35416666666666669</v>
+        <v>0.35555555555555557</v>
       </c>
       <c r="F19" s="8">
         <v>0.45833333333333331</v>
@@ -6178,35 +6524,31 @@
       <c r="K19" t="s">
         <v>80</v>
       </c>
+      <c r="L19" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>230801</v>
+        <v>230728</v>
       </c>
       <c r="B20" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8">
-        <v>0.54305555555555551</v>
-      </c>
-      <c r="G20" s="8">
-        <v>0.55763888888888891</v>
-      </c>
-      <c r="H20" s="8">
-        <v>0.56597222222222221</v>
-      </c>
-      <c r="J20" s="8">
-        <v>0.625</v>
+        <v>14</v>
+      </c>
+      <c r="D20" s="8">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="F20" s="8">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="I20" s="8">
+        <v>0.4861111111111111</v>
       </c>
       <c r="K20" t="s">
-        <v>85</v>
-      </c>
-      <c r="L20" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.35">
@@ -6214,14 +6556,14 @@
         <v>230801</v>
       </c>
       <c r="B21" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D21" s="8"/>
       <c r="E21" s="8">
-        <v>0.54375000000000007</v>
+        <v>0.54305555555555551</v>
       </c>
       <c r="G21" s="8">
         <v>0.55763888888888891</v>
@@ -6230,34 +6572,40 @@
         <v>0.56597222222222221</v>
       </c>
       <c r="J21" s="8">
-        <v>0.63402777777777775</v>
+        <v>0.625</v>
       </c>
       <c r="K21" t="s">
         <v>85</v>
       </c>
+      <c r="L21" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>230802</v>
+        <v>230801</v>
       </c>
       <c r="B22" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8">
-        <v>0.44930555555555557</v>
+        <v>0.54375000000000007</v>
+      </c>
+      <c r="G22" s="8">
+        <v>0.55763888888888891</v>
+      </c>
+      <c r="H22" s="8">
+        <v>0.56597222222222221</v>
       </c>
       <c r="J22" s="8">
-        <v>0.4548611111111111</v>
+        <v>0.63402777777777775</v>
       </c>
       <c r="K22" t="s">
-        <v>88</v>
-      </c>
-      <c r="L22" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.35">
@@ -6265,25 +6613,28 @@
         <v>230802</v>
       </c>
       <c r="B23" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D23" s="8"/>
       <c r="E23" s="8">
-        <v>0.43194444444444446</v>
+        <v>0.44930555555555557</v>
       </c>
       <c r="J23" s="8">
-        <v>0.44930555555555557</v>
+        <v>0.4548611111111111</v>
       </c>
       <c r="K23" t="s">
         <v>88</v>
       </c>
+      <c r="L23" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>230804</v>
+        <v>230802</v>
       </c>
       <c r="B24" s="3">
         <v>5</v>
@@ -6291,18 +6642,15 @@
       <c r="C24" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="D24" s="8"/>
       <c r="E24" s="8">
-        <v>0.38958333333333334</v>
-      </c>
-      <c r="I24" s="8"/>
+        <v>0.43194444444444446</v>
+      </c>
       <c r="J24" s="8">
-        <v>0.40138888888888885</v>
+        <v>0.44930555555555557</v>
       </c>
       <c r="K24" t="s">
         <v>88</v>
-      </c>
-      <c r="L24" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.35">
@@ -6310,25 +6658,28 @@
         <v>230804</v>
       </c>
       <c r="B25" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E25" s="8">
-        <v>0.40138888888888885</v>
+        <v>0.38958333333333334</v>
       </c>
       <c r="I25" s="8"/>
       <c r="J25" s="8">
-        <v>0.4055555555555555</v>
+        <v>0.40138888888888885</v>
       </c>
       <c r="K25" t="s">
         <v>88</v>
       </c>
+      <c r="L25" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26">
-        <v>230807</v>
+        <v>230804</v>
       </c>
       <c r="B26" s="3">
         <v>3</v>
@@ -6336,32 +6687,15 @@
       <c r="C26" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="8">
-        <v>0.60972222222222217</v>
-      </c>
       <c r="E26" s="8">
-        <v>0.60972222222222217</v>
-      </c>
-      <c r="F26" s="8">
-        <v>0.63055555555555554</v>
-      </c>
-      <c r="G26" s="8">
-        <v>0.65277777777777779</v>
-      </c>
-      <c r="H26" s="8">
-        <v>0.67013888888888884</v>
-      </c>
-      <c r="I26" s="8">
-        <v>0.69444444444444453</v>
-      </c>
+        <v>0.40138888888888885</v>
+      </c>
+      <c r="I26" s="8"/>
       <c r="J26" s="8">
-        <v>0.68958333333333333</v>
+        <v>0.4055555555555555</v>
       </c>
       <c r="K26" t="s">
         <v>88</v>
-      </c>
-      <c r="L26" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.35">
@@ -6369,34 +6703,159 @@
         <v>230807</v>
       </c>
       <c r="B27" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D27" s="8">
-        <v>0.6118055555555556</v>
+        <v>0.60972222222222217</v>
       </c>
       <c r="E27" s="8">
-        <v>0.6118055555555556</v>
+        <v>0.60972222222222217</v>
       </c>
       <c r="F27" s="8">
         <v>0.63055555555555554</v>
       </c>
       <c r="G27" s="8">
-        <v>0.64236111111111105</v>
+        <v>0.65277777777777779</v>
       </c>
       <c r="H27" s="8">
-        <v>0.66041666666666665</v>
+        <v>0.67013888888888884</v>
       </c>
       <c r="I27" s="8">
         <v>0.69444444444444453</v>
       </c>
       <c r="J27" s="8">
-        <v>0.68680555555555556</v>
+        <v>0.68958333333333333</v>
       </c>
       <c r="K27" t="s">
         <v>88</v>
+      </c>
+      <c r="L27" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>230807</v>
+      </c>
+      <c r="B28" s="3">
+        <v>5</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" s="8">
+        <v>0.6118055555555556</v>
+      </c>
+      <c r="E28" s="8">
+        <v>0.6118055555555556</v>
+      </c>
+      <c r="F28" s="8">
+        <v>0.63055555555555554</v>
+      </c>
+      <c r="G28" s="8">
+        <v>0.64236111111111105</v>
+      </c>
+      <c r="H28" s="8">
+        <v>0.66041666666666665</v>
+      </c>
+      <c r="I28" s="8">
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="J28" s="8">
+        <v>0.68680555555555556</v>
+      </c>
+      <c r="K28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>230821</v>
+      </c>
+      <c r="B29" s="3">
+        <v>5</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="8">
+        <v>0.44513888888888892</v>
+      </c>
+      <c r="E29" s="8">
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="F29" s="8">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="J29" s="8">
+        <v>0.5493055555555556</v>
+      </c>
+      <c r="K29" t="s">
+        <v>88</v>
+      </c>
+      <c r="L29" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>230821</v>
+      </c>
+      <c r="B30" s="3">
+        <v>3</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D30" s="8">
+        <v>0.44861111111111113</v>
+      </c>
+      <c r="E30" s="8">
+        <v>0.44722222222222219</v>
+      </c>
+      <c r="F30" s="8">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="I30" s="8">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="J30" s="8">
+        <v>0.55347222222222225</v>
+      </c>
+      <c r="K30" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>230822</v>
+      </c>
+      <c r="B31" s="3">
+        <v>3</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="J31" s="8">
+        <v>0.42152777777777778</v>
+      </c>
+      <c r="K31" t="s">
+        <v>88</v>
+      </c>
+      <c r="L31" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -6409,7 +6868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{219CC811-8442-4429-81C5-6ADB9C52A9AC}">
   <dimension ref="A1:N92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>

</xml_diff>